<commit_message>
Update core to building Cucumber
</commit_message>
<xml_diff>
--- a/src/test/resources/testdatafile/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdatafile/ClientsDataExcel.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdatafile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkCucumberTestNG\src\test\resources\testdatafile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565D20AF-727F-45C0-A90B-DEBCE91B4E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD2A4C4-009A-432D-8726-532480955C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="1776" windowWidth="18600" windowHeight="10224" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
@@ -18,27 +18,15 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
-  <si>
-    <t>Admin Anh Tester</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Dong Thap</t>
   </si>
@@ -67,9 +55,6 @@
     <t>O Mon</t>
   </si>
   <si>
-    <t>Team Leader 01</t>
-  </si>
-  <si>
     <t>T+wyT5u9cOelDJbBWNgxLw==</t>
   </si>
   <si>
@@ -91,83 +76,94 @@
     <t>manual</t>
   </si>
   <si>
+    <t>TESTCASENAME</t>
+  </si>
+  <si>
+    <t>OWNER</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>WEBSITE</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>COMPANY_NAME</t>
+  </si>
+  <si>
+    <t>CLIENT_GROUP</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>EXPECTED_TITLE</t>
+  </si>
+  <si>
+    <t>EXPECTED_ERROR</t>
+  </si>
+  <si>
+    <t>EXPECTED_URL</t>
+  </si>
+  <si>
+    <t>admin02@mailinator.com</t>
+  </si>
+  <si>
+    <t>tld01@mailinator.com</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>testGetSignInData</t>
+  </si>
+  <si>
     <t>testAddClient</t>
   </si>
   <si>
-    <t>TESTCASENAME</t>
-  </si>
-  <si>
-    <t>OWNER</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>CITY</t>
-  </si>
-  <si>
-    <t>STATE</t>
-  </si>
-  <si>
-    <t>ZIP</t>
-  </si>
-  <si>
-    <t>COUNTRY</t>
-  </si>
-  <si>
-    <t>PHONE</t>
-  </si>
-  <si>
-    <t>WEBSITE</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>COMPANY_NAME</t>
-  </si>
-  <si>
-    <t>CLIENT_GROUP</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>EXPECTED_TITLE</t>
-  </si>
-  <si>
-    <t>EXPECTED_ERROR</t>
-  </si>
-  <si>
-    <t>EXPECTED_URL</t>
-  </si>
-  <si>
-    <t>testSignInTest</t>
-  </si>
-  <si>
-    <t>admin02@mailinator.com</t>
-  </si>
-  <si>
-    <t>tld01@mailinator.com</t>
-  </si>
-  <si>
-    <t>Anh Tester Com 2204</t>
-  </si>
-  <si>
-    <t>Anh Tester Com 3004</t>
-  </si>
-  <si>
-    <t>pass</t>
+    <t>Thai Thi Hanh</t>
+  </si>
+  <si>
+    <t>Admin 02</t>
+  </si>
+  <si>
+    <t>Team Member 01</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 1506A1</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 1506A2</t>
+  </si>
+  <si>
+    <t>Anh Tester Client 1506A3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,11 +266,6 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="11"/>
       </patternFill>
     </fill>
     <fill>
@@ -333,7 +324,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -651,42 +642,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="12" width="18.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="12" width="30.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="12" width="33.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="12" width="18.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="12" width="20.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="12" width="17.33203125" collapsed="true"/>
-    <col min="7" max="8" style="12" width="8.88671875" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="21.6640625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.33203125" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.21875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.44140625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.77734375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="8.88671875" style="12" collapsed="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -694,13 +685,13 @@
         <v>36</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s" s="14">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -708,10 +699,10 @@
         <v>36</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -726,155 +717,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E2E380-41FF-438A-822D-1CBE2A443631}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="18.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="23.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="19.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="11.44140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="14.44140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="24.5546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="5.33203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="16.21875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="9.109375" collapsed="true"/>
-    <col min="14" max="16384" style="2" width="18.21875" collapsed="true"/>
+    <col min="1" max="1" width="18.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.21875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.21875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.21875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="18.21875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="J2" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>90000</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3">
+        <v>30</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="6"/>
+      <c r="M4" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{ED197778-D3E0-411D-9BE8-9D641596BB30}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{6BB180CC-F100-4639-BD3A-B7B33CC640F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>